<commit_message>
Fixed colors on excel sheet
</commit_message>
<xml_diff>
--- a/board.xlsx
+++ b/board.xlsx
@@ -223,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,11 +588,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,7 +939,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J8" sqref="J8:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,25 +1469,25 @@
       <c r="I8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="3" t="s">
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -1533,25 +1540,25 @@
       <c r="I9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="3" t="s">
+      <c r="J9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Q9" s="1" t="s">
@@ -1604,25 +1611,25 @@
       <c r="I10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="3" t="s">
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Q10" s="1" t="s">
@@ -1675,25 +1682,25 @@
       <c r="I11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P11" s="3" t="s">
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Q11" s="1" t="s">
@@ -1746,25 +1753,25 @@
       <c r="I12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="3" t="s">
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="Q12" s="1" t="s">

</xml_diff>

<commit_message>
Added Failing tests for adjacency/target calculations which handle for doors...etc
</commit_message>
<xml_diff>
--- a/board.xlsx
+++ b/board.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="board" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="32">
   <si>
     <t>C</t>
   </si>
@@ -80,6 +80,36 @@
   </si>
   <si>
     <t>DR</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>testAdjacenciesInsideRoom</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>testAdjacencyRoomExit</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>testAdjacencyWalkways</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>testAdjacencyDoorways</t>
+  </si>
+  <si>
+    <t>Light Blue</t>
+  </si>
+  <si>
+    <t>testTargets targets</t>
   </si>
 </sst>
 </file>
@@ -223,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +454,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,12 +648,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -936,16 +1002,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:P12"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -957,7 +1023,7 @@
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1229,7 +1295,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1241,7 +1307,7 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1256,7 +1322,7 @@
       <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -1289,7 +1355,7 @@
       <c r="T5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="U5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="V5" s="3" t="s">
@@ -1345,7 +1411,7 @@
       <c r="O6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -1360,7 +1426,7 @@
       <c r="T6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1371,7 +1437,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1416,7 +1482,7 @@
       <c r="O7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="Q7" s="1" t="s">
@@ -1434,7 +1500,7 @@
       <c r="U7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="W7" s="1" t="s">
@@ -1502,7 +1568,7 @@
       <c r="T8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="V8" s="3" t="s">
@@ -1706,7 +1772,7 @@
       <c r="Q11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S11" s="3" t="s">
@@ -1744,7 +1810,7 @@
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1818,7 +1884,7 @@
       <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1939,7 +2005,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1993,20 +2059,20 @@
       <c r="R15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>18</v>
+      <c r="S15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2031,7 +2097,7 @@
       <c r="G16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2061,16 +2127,16 @@
       <c r="Q16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>18</v>
+      <c r="R16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U16" s="3" t="s">
+      <c r="U16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="V16" s="3" t="s">
@@ -2200,7 +2266,7 @@
       <c r="P18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -2256,7 +2322,7 @@
       <c r="K19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M19" s="3" t="s">
@@ -2457,7 +2523,7 @@
       <c r="G22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -2481,7 +2547,7 @@
       <c r="O22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P22" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Q22" s="1" t="s">
@@ -2504,9 +2570,53 @@
       </c>
       <c r="W22" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V23" s="10"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>